<commit_message>
refactor: Remove unused functions
- Removed load_result() and print_history() from results_manager.py
- Removed compute_prototype_assignment_loss() from clustering_loss.py
- Removed get_dataset_info() from dataset_utils.py
- Total: ~100 lines of dead code removed
- Cleaner codebase with only actively used functions
</commit_message>
<xml_diff>
--- a/results/comparison_table.xlsx
+++ b/results/comparison_table.xlsx
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>0.4399</v>
+        <v>0.4348</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>0.8542</v>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>0.7667</v>
+        <v>0.75</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>0.9167</v>
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0.965</v>
+        <v>0.9592000000000001</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>0.9825</v>
@@ -741,20 +741,20 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
+        <v>0.8929</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>0.9643</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="n">
+      <c r="F5" s="6" t="n">
         <v>0.9643</v>
       </c>
-      <c r="F5" s="4" t="n">
-        <v>0.9643</v>
-      </c>
       <c r="G5" s="5" t="n">
         <v>1</v>
       </c>
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>2.5</v>
@@ -771,10 +771,10 @@
         <v>2.5</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="N5" s="6" t="n">
         <v>2.5</v>
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>0.9213</v>
+        <v>0.9314</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0.9621</v>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0.9409</v>
+        <v>0.9402</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0.9681999999999999</v>
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>0.9733000000000001</v>
+        <v>0.9467</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>1</v>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>0.7143</v>
+        <v>0.6381</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>0.8286</v>
@@ -958,7 +958,7 @@
         <v>0.4667</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>1</v>
@@ -970,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N9" s="6" t="n">
         <v>2</v>
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>0.5833</v>
+        <v>0.55</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0.9833</v>
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>0.54</v>
+        <v>0.58</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>0.76</v>

</xml_diff>